<commit_message>
add test for the importService
</commit_message>
<xml_diff>
--- a/src/test/resources/test_missing_class_code_header_file.xlsx
+++ b/src/test/resources/test_missing_class_code_header_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ttzhang/Documents/projects/Natlex_Task/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE99C880-F101-E446-B4AF-E0DC277CC580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC465A45-2EC5-FD45-BE03-E3B6950E7217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20660" xr2:uid="{C461ED32-CABF-9343-80F3-C9D876E969B0}"/>
   </bookViews>
@@ -36,99 +36,70 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t xml:space="preserve">Class 2 name </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Class 2 code </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Section 1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geo Class 11 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GC11 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geo Class 12 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GC12 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Section 2 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geo Class 21 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GC21 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geo Class 22 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GC22 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Section 3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geo Class 31 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GC31 </t>
-  </si>
-  <si>
-    <t>Section 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geo Class 41 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GC41 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geo Class 42 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geo Class 32 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GC32 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GC42 </t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>Section Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Class 1 name </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>Section 1</t>
+  </si>
+  <si>
+    <t>Section 2</t>
+  </si>
+  <si>
+    <t>Section 3</t>
+  </si>
+  <si>
+    <t>Geo Class 11</t>
+  </si>
+  <si>
+    <t>GC11</t>
+  </si>
+  <si>
+    <t>Geo Class 12</t>
+  </si>
+  <si>
+    <t>GC12</t>
+  </si>
+  <si>
+    <t>Geo Class 21</t>
+  </si>
+  <si>
+    <t>GC21</t>
+  </si>
+  <si>
+    <t>Geo Class 22</t>
+  </si>
+  <si>
+    <t>GC22</t>
+  </si>
+  <si>
+    <t>GC32</t>
+  </si>
+  <si>
+    <t>Geo Class 32</t>
+  </si>
+  <si>
+    <t>Section name</t>
+  </si>
+  <si>
+    <t>Class 1 name</t>
+  </si>
+  <si>
+    <t>Class 2 name</t>
+  </si>
+  <si>
+    <t>Class 2 code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="2">
@@ -151,9 +122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -489,204 +458,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A30A9BAD-409A-184F-A9F9-B12D7A9A0BC3}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.5" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="27.33203125" customWidth="1"/>
-    <col min="4" max="4" width="27.6640625" customWidth="1"/>
-    <col min="5" max="5" width="25.6640625" customWidth="1"/>
-    <col min="6" max="6" width="50.5" customWidth="1"/>
-    <col min="7" max="7" width="23" customWidth="1"/>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
         <v>11</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>